<commit_message>
different logic for buyer's market choice
</commit_message>
<xml_diff>
--- a/input/input.xlsx
+++ b/input/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pleger/Documents/Projects/ChinaSimulatioN_V2/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19E17FE-C847-5148-B8E7-29145F0A15C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AE1E5E-9AB5-C349-A948-9982C0DB54E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25000" windowHeight="12580" xr2:uid="{B078D86E-CB7D-D145-8E1E-BF1E3C336D06}"/>
+    <workbookView xWindow="15200" yWindow="1360" windowWidth="28700" windowHeight="12580" xr2:uid="{B078D86E-CB7D-D145-8E1E-BF1E3C336D06}"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>Variables</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>REPETITIONS</t>
+  </si>
+  <si>
+    <t>MEMORY</t>
   </si>
 </sst>
 </file>
@@ -654,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{907F1E5B-209D-BA4A-9A57-BB6890C684CF}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -670,7 +673,7 @@
         <v>31</v>
       </c>
       <c r="B1">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -678,15 +681,15 @@
         <v>22</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B3">
-        <v>17</v>
+      <c r="B3" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -734,7 +737,7 @@
         <v>28</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -743,6 +746,14 @@
       </c>
       <c r="B10">
         <v>1.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -755,7 +766,9 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView zoomScale="99" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:M2"/>
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A2" sqref="A2"/>
+      <selection pane="topRight" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>